<commit_message>
Added code to read categories from Excel at the start for better
condition checking
</commit_message>
<xml_diff>
--- a/src/test/resources/CategoryPrices.xlsx
+++ b/src/test/resources/CategoryPrices.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="2" r:id="rId1"/>
+    <sheet name="ManualCheck" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>TOI</t>
   </si>
@@ -53,6 +54,15 @@
   </si>
   <si>
     <t>Sunday</t>
+  </si>
+  <si>
+    <t>Year/Month</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>2020, Apr</t>
   </si>
 </sst>
 </file>
@@ -605,4 +615,174 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1">
+        <f>SUM(I:I)</f>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="1">
+        <f>B4*$B$2+C4*$C$2+D4*$D$2+E4*$E$2+F4*$F$2+G4*$G$2+H4*$H$2</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <f>B5*$B$2+C5*$C$2+D5*$D$2+E5*$E$2+F5*$F$2+G5*$G$2+H5*$H$2</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <f>B6*$B$2+C6*$C$2+D6*$D$2+E6*$E$2+F6*$F$2+G6*$G$2+H6*$H$2</f>
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Caught a bug in PrototypeTwoTest related to incorrect calculation of
Subscription amount and made necessary change.
</commit_message>
<xml_diff>
--- a/src/test/resources/CategoryPrices.xlsx
+++ b/src/test/resources/CategoryPrices.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>TOI</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>2020, Apr</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Magazine</t>
+  </si>
+  <si>
+    <t>Carwash</t>
+  </si>
+  <si>
+    <t>Biweekly</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Weekly</t>
   </si>
 </sst>
 </file>
@@ -127,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +154,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -442,11 +466,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -611,6 +633,84 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4">
+        <v>50</v>
+      </c>
+      <c r="D7" s="4">
+        <v>50</v>
+      </c>
+      <c r="E7" s="4">
+        <v>50</v>
+      </c>
+      <c r="F7" s="4">
+        <v>50</v>
+      </c>
+      <c r="G7" s="4">
+        <v>50</v>
+      </c>
+      <c r="H7" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>150</v>
+      </c>
+      <c r="C8" s="4">
+        <v>150</v>
+      </c>
+      <c r="D8" s="4">
+        <v>150</v>
+      </c>
+      <c r="E8" s="4">
+        <v>150</v>
+      </c>
+      <c r="F8" s="4">
+        <v>150</v>
+      </c>
+      <c r="G8" s="4">
+        <v>150</v>
+      </c>
+      <c r="H8" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>200</v>
+      </c>
+      <c r="C9" s="4">
+        <v>200</v>
+      </c>
+      <c r="D9" s="4">
+        <v>200</v>
+      </c>
+      <c r="E9" s="4">
+        <v>200</v>
+      </c>
+      <c r="F9" s="4">
+        <v>200</v>
+      </c>
+      <c r="G9" s="4">
+        <v>200</v>
+      </c>
+      <c r="H9" s="4">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -619,11 +719,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -633,7 +731,7 @@
     <col min="7" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -658,15 +756,15 @@
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1">
+      <c r="L1" s="5">
         <f>SUM(I:I)</f>
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2731</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -692,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -722,7 +820,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +850,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -780,6 +878,39 @@
       <c r="I6" s="1">
         <f>B6*$B$2+C6*$C$2+D6*$D$2+E6*$E$2+F6*$F$2+G6*$G$2+H6*$H$2</f>
         <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1">
+        <v>400</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1">
+        <v>600</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sample output to CategoryPrices excel under src/test/resources
</commit_message>
<xml_diff>
--- a/src/test/resources/CategoryPrices.xlsx
+++ b/src/test/resources/CategoryPrices.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6015" tabRatio="813"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="2" r:id="rId1"/>
     <sheet name="ManualCheck" sheetId="3" r:id="rId2"/>
+    <sheet name="PrototypeOneTest output" sheetId="5" r:id="rId3"/>
+    <sheet name="PrototypeTwoTest output" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <oleSize ref="A1:N18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>TOI</t>
   </si>
@@ -81,6 +84,90 @@
   </si>
   <si>
     <t>Weekly</t>
+  </si>
+  <si>
+    <t>Enter category followed by frequency whose subscription needs to be calculated. Choices are :: [Hindu, Carwash, BM, HT, Magazine, TOI, ET, Milk]</t>
+  </si>
+  <si>
+    <t>The input to the program should be a comma separated list of categories that the consumer wants to subscribe followed by Daily,Weekly,Biweekly (eg: TOI,Daily,ET,Weekly,HM,BiWeekly)</t>
+  </si>
+  <si>
+    <t>Enter your string here :: BM,Daily,BM,Daily,ET,Blah,Blah,Weekly,HT,Daily,TOI,Daily,Milk,Daily,Magazine,Weekly,Carwash,Biweekly</t>
+  </si>
+  <si>
+    <t>{Carwash=Biweekly, BM=Daily, HT=Daily, Magazine=Weekly, TOI=Daily, Milk=Daily}</t>
+  </si>
+  <si>
+    <t>*******************************************************************</t>
+  </si>
+  <si>
+    <t>Enter the Year followed by Month (using first three letters only) seperated by comma whose budget needs calculated (eg: 2020,Mar) :: 2020,Apr</t>
+  </si>
+  <si>
+    <t>Total number of days in the Month 'Apr' and Year '2020' is :: 30</t>
+  </si>
+  <si>
+    <t>{Monday=4, Thursday=5, Friday=4, Sunday=4, Wednesday=5, Tuesday=4, Saturday=4}</t>
+  </si>
+  <si>
+    <t>Calculation Table for 'Carwash' is :: {Monday=200.0, Thursday=200.0, Friday=200.0, Sunday=200.0, Wednesday=200.0, Tuesday=200.0, Saturday=200.0}</t>
+  </si>
+  <si>
+    <t>Total Biweekly subscription for Carwash is Rs 200.0</t>
+  </si>
+  <si>
+    <t>Therefore, total monthly subscription for Carwash is Rs 400.0</t>
+  </si>
+  <si>
+    <t>Calculation Table for 'BM' is :: {Monday=1.5, Thursday=1.5, Friday=1.5, Sunday=1.5, Wednesday=1.5, Tuesday=1.5, Saturday=1.5}</t>
+  </si>
+  <si>
+    <t>Total Monthly subscription for BM is Rs 45.0</t>
+  </si>
+  <si>
+    <t>Calculation Table for 'HT' is :: {Monday=2.0, Thursday=2.0, Friday=2.0, Sunday=4.0, Wednesday=2.0, Tuesday=2.0, Saturday=4.0}</t>
+  </si>
+  <si>
+    <t>Total Monthly subscription for HT is Rs 76.0</t>
+  </si>
+  <si>
+    <t>Calculation Table for 'Magazine' is :: {Monday=150.0, Thursday=150.0, Friday=150.0, Sunday=150.0, Wednesday=150.0, Tuesday=150.0, Saturday=150.0}</t>
+  </si>
+  <si>
+    <t>Total Weekly subscription for Magazine is Rs 150.0</t>
+  </si>
+  <si>
+    <t>Therefore, total Monthly subscription for Magazine is Rs 600.0</t>
+  </si>
+  <si>
+    <t>Calculation Table for 'TOI' is :: {Monday=3.0, Thursday=3.0, Friday=3.0, Sunday=6.0, Wednesday=3.0, Tuesday=3.0, Saturday=5.0}</t>
+  </si>
+  <si>
+    <t>Total Monthly subscription for TOI is Rs 110.0</t>
+  </si>
+  <si>
+    <t>Calculation Table for 'Milk' is :: {Monday=50.0, Thursday=50.0, Friday=50.0, Sunday=50.0, Wednesday=50.0, Tuesday=50.0, Saturday=50.0}</t>
+  </si>
+  <si>
+    <t>Total Monthly subscription for Milk is Rs 1500.0</t>
+  </si>
+  <si>
+    <t>Total estimated subscription amount for the month of 'Apr' and year '2020' is  :: Rs 2731.0</t>
+  </si>
+  <si>
+    <t>Enter Newspaper whose monthly subscription needs to be calculated. Choices are :: [Hindu, Carwash, BM, HT, Magazine, TOI, ET, Milk]</t>
+  </si>
+  <si>
+    <t>The input to the program should be a comma separated list of papers that the consumer wants to subscribe (eg: TOI,ET)</t>
+  </si>
+  <si>
+    <t>Enter your string here :: TOI,BM,HT,Random,TOI,Random,BM,@#@$,BM</t>
+  </si>
+  <si>
+    <t>[BM, HT, TOI]</t>
+  </si>
+  <si>
+    <t>Total estimated subscription amount for the month of 'Apr' and year '2020' is  :: Rs 231.0</t>
   </si>
 </sst>
 </file>
@@ -916,4 +1003,260 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed CategoryPrices.xlsx to align with ProtoTypeOne
</commit_message>
<xml_diff>
--- a/src/test/resources/CategoryPrices.xlsx
+++ b/src/test/resources/CategoryPrices.xlsx
@@ -13,12 +13,11 @@
     <sheet name="PrototypeTwoTest output" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <oleSize ref="A1:N18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>TOI</t>
   </si>
@@ -232,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,9 +240,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -553,9 +549,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -720,84 +718,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2">
-        <v>50</v>
-      </c>
-      <c r="C7" s="4">
-        <v>50</v>
-      </c>
-      <c r="D7" s="4">
-        <v>50</v>
-      </c>
-      <c r="E7" s="4">
-        <v>50</v>
-      </c>
-      <c r="F7" s="4">
-        <v>50</v>
-      </c>
-      <c r="G7" s="4">
-        <v>50</v>
-      </c>
-      <c r="H7" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2">
-        <v>150</v>
-      </c>
-      <c r="C8" s="4">
-        <v>150</v>
-      </c>
-      <c r="D8" s="4">
-        <v>150</v>
-      </c>
-      <c r="E8" s="4">
-        <v>150</v>
-      </c>
-      <c r="F8" s="4">
-        <v>150</v>
-      </c>
-      <c r="G8" s="4">
-        <v>150</v>
-      </c>
-      <c r="H8" s="4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2">
-        <v>200</v>
-      </c>
-      <c r="C9" s="4">
-        <v>200</v>
-      </c>
-      <c r="D9" s="4">
-        <v>200</v>
-      </c>
-      <c r="E9" s="4">
-        <v>200</v>
-      </c>
-      <c r="F9" s="4">
-        <v>200</v>
-      </c>
-      <c r="G9" s="4">
-        <v>200</v>
-      </c>
-      <c r="H9" s="4">
-        <v>200</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -808,7 +728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -843,10 +765,10 @@
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="4">
         <f>SUM(I:I)</f>
         <v>2731</v>
       </c>
@@ -1033,13 +955,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
@@ -1055,13 +975,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
@@ -1072,7 +990,6 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
@@ -1083,7 +1000,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
@@ -1094,14 +1010,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
@@ -1145,7 +1058,6 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
@@ -1161,13 +1073,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
@@ -1183,7 +1093,6 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
@@ -1194,7 +1103,6 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
@@ -1205,7 +1113,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
@@ -1221,7 +1128,6 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
@@ -1232,7 +1138,6 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
@@ -1243,14 +1148,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>

</xml_diff>